<commit_message>
Updates to tissue calculations
</commit_message>
<xml_diff>
--- a/VQC R work/Data Sheets/PFAS_Rdata_Tissue.xlsx
+++ b/VQC R work/Data Sheets/PFAS_Rdata_Tissue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://keckmedicine-my.sharepoint.com/personal/victoria_quonchow_med_usc_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victoriaqc/Documents/GitHub/PFAS_met_cage/VQC R work/Data Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07089F4B-589A-D34E-B400-BD44BF2734F4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E074C92D-F7AD-5F40-878C-4B9227C7525F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="3880" windowWidth="28740" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="6000" windowWidth="28740" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Right_Kidney</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Heart_Weight</t>
+  </si>
+  <si>
+    <t>HW_BW_In</t>
+  </si>
+  <si>
+    <t>KW_BW_In</t>
   </si>
 </sst>
 </file>
@@ -428,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -444,7 +450,7 @@
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -466,8 +472,14 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3920</v>
       </c>
@@ -489,8 +501,14 @@
       <c r="G2">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I2">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3921</v>
       </c>
@@ -512,8 +530,14 @@
       <c r="G3">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>4.3</v>
+      </c>
+      <c r="I3">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3922</v>
       </c>
@@ -535,8 +559,14 @@
       <c r="G4">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>4.3</v>
+      </c>
+      <c r="I4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3923</v>
       </c>
@@ -558,8 +588,14 @@
       <c r="G5">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I5">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3932</v>
       </c>
@@ -581,8 +617,14 @@
       <c r="G6">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>4.2</v>
+      </c>
+      <c r="I6">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3933</v>
       </c>
@@ -604,8 +646,14 @@
       <c r="G7">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>4.3</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3934</v>
       </c>
@@ -627,8 +675,14 @@
       <c r="G8">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>5.4</v>
+      </c>
+      <c r="I8">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3935</v>
       </c>
@@ -650,8 +704,14 @@
       <c r="G9">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>4.2</v>
+      </c>
+      <c r="I9">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3936</v>
       </c>
@@ -673,8 +733,14 @@
       <c r="G10">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3937</v>
       </c>
@@ -696,8 +762,14 @@
       <c r="G11">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>2.8</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3938</v>
       </c>
@@ -719,8 +791,14 @@
       <c r="G12">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>3.3</v>
+      </c>
+      <c r="I12">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3939</v>
       </c>
@@ -741,6 +819,12 @@
       </c>
       <c r="G13">
         <v>4.3</v>
+      </c>
+      <c r="H13">
+        <v>3.1</v>
+      </c>
+      <c r="I13">
+        <v>10.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>